<commit_message>
Ahora los índices de punteo se reasignan en orden secuencial sin alterar el orden de las filas. Si necesitas más ajustes, dime.
</commit_message>
<xml_diff>
--- a/informes/Puntear/Puntear_no_punteados.xlsx
+++ b/informes/Puntear/Puntear_no_punteados.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,156 +440,162 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>F.Mov.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Num. As.</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tercero</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Nom. Tercero</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Debe</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Haber</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Cuadra</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Cuenta</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Cuenta M/F</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo.Mov</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo de 3º</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Documento</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>Indice_Punteo</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>F.Mov.</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Num. As.</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Comentario</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Tercero</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Nom. Tercero</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Debe</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Haber</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Usuario</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Cuadra</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Cuenta</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Cuenta M/F</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo.Mov</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo de 3º</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Documento</t>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Indice_Punteo</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" s="2" t="n">
+      <c r="A2" s="2" t="n">
         <v>45656</v>
       </c>
-      <c r="C2" t="n">
+      <c r="B2" t="n">
         <v>4047697</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Creación Anticipo 409127725/1</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>4824</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>IMEDISA ARTES GRAFICAS, S.L.U.</t>
         </is>
       </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" t="n">
+        <v>738.84</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-738.84</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="n">
-        <v>738.84</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-738.84</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>sandra</t>
+        </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>sandra</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="L2" t="n">
         <v>438004824</v>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>N</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
           <t>409127725/1</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>